<commit_message>
return book page + other excel file types supported
</commit_message>
<xml_diff>
--- a/static/files/students_chart.xlsx
+++ b/static/files/students_chart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Judáš</t>
   </si>
   <si>
-    <t>Betka</t>
-  </si>
-  <si>
     <t>Hanna</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t xml:space="preserve">Robo </t>
   </si>
   <si>
-    <t xml:space="preserve">Samo </t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -69,22 +63,22 @@
     <t>Septima</t>
   </si>
   <si>
-    <t>Oktáva</t>
-  </si>
-  <si>
-    <t>Príma</t>
-  </si>
-  <si>
     <t>Tercia</t>
   </si>
   <si>
     <t>3.B</t>
   </si>
   <si>
-    <t>I.A</t>
-  </si>
-  <si>
-    <t>2.A</t>
+    <t>1.A</t>
+  </si>
+  <si>
+    <t>Ľumi</t>
+  </si>
+  <si>
+    <t>Prima</t>
+  </si>
+  <si>
+    <t>Oktava</t>
   </si>
 </sst>
 </file>
@@ -430,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="M17" sqref="M17:Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -446,10 +440,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -463,7 +457,7 @@
         <v>111111</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -477,7 +471,7 @@
         <v>222222</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -491,7 +485,7 @@
         <v>333333</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -505,7 +499,7 @@
         <v>444444</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -513,13 +507,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>555555</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -533,7 +527,7 @@
         <v>666666</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -541,13 +535,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>777777</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -555,13 +549,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>888888</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -569,27 +563,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>999999</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11">
-        <v>1111110</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>